<commit_message>
Added Description, wrapper functionality, and saving data
</commit_message>
<xml_diff>
--- a/data analysis/Alphapower_SNR.xlsx
+++ b/data analysis/Alphapower_SNR.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Oz</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t>SNR 80 psycho</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>KSS</t>
+  </si>
+  <si>
+    <t>Avg O</t>
   </si>
 </sst>
 </file>
@@ -204,10 +213,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>22</c:v>
                 </c:pt>
@@ -222,16 +231,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11.41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>6.7199999999999996E-2</c:v>
                 </c:pt>
@@ -246,6 +258,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.14549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0999999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -279,10 +294,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>22</c:v>
                 </c:pt>
@@ -297,16 +312,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11.41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>9.01E-2</c:v>
                 </c:pt>
@@ -321,6 +339,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.13389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4200000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -354,10 +375,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>22</c:v>
                 </c:pt>
@@ -372,16 +393,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11.41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.77E-2</c:v>
                 </c:pt>
@@ -396,6 +420,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4.4900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -410,11 +437,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="477366304"/>
-        <c:axId val="452190632"/>
+        <c:axId val="189958368"/>
+        <c:axId val="189958760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="477366304"/>
+        <c:axId val="189958368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,12 +498,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="452190632"/>
+        <c:crossAx val="189958760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="452190632"/>
+        <c:axId val="189958760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -533,7 +560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477366304"/>
+        <c:crossAx val="189958368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -717,10 +744,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$F$8</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>18.82</c:v>
                 </c:pt>
@@ -735,16 +762,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>6.7199999999999996E-2</c:v>
                 </c:pt>
@@ -759,6 +789,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.14549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0999999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -792,10 +825,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$F$8</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>18.82</c:v>
                 </c:pt>
@@ -810,16 +843,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>9.01E-2</c:v>
                 </c:pt>
@@ -834,6 +870,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.13389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4200000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -867,10 +906,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$F$8</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>18.82</c:v>
                 </c:pt>
@@ -885,16 +924,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.77E-2</c:v>
                 </c:pt>
@@ -909,6 +951,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4.4900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,11 +968,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226469944"/>
-        <c:axId val="168343848"/>
+        <c:axId val="189960720"/>
+        <c:axId val="189960328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226469944"/>
+        <c:axId val="189960720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -984,12 +1029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="168343848"/>
+        <c:crossAx val="189960328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="168343848"/>
+        <c:axId val="189960328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1091,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226469944"/>
+        <c:crossAx val="189960720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1230,10 +1275,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$F$8</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>18.82</c:v>
                 </c:pt>
@@ -1248,16 +1293,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.77E-2</c:v>
                 </c:pt>
@@ -1272,6 +1320,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4.4900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,11 +1337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="473203032"/>
-        <c:axId val="473201856"/>
+        <c:axId val="189957584"/>
+        <c:axId val="100512888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="473203032"/>
+        <c:axId val="189957584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,12 +1398,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473201856"/>
+        <c:crossAx val="100512888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="473201856"/>
+        <c:axId val="100512888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,7 +1460,425 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473203032"/>
+        <c:crossAx val="189957584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Occipital Alpha power vs SNR</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>18.82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.8333333333333327E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.376666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17519999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16523333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.606666666666667E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.8333333333333327E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.376666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17519999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16523333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.606666666666667E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="105381424"/>
+        <c:axId val="105381032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="105381424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105381032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="105381032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105381424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1578,6 +2047,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2611,6 +3120,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3193,15 +4218,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3215,6 +4240,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3486,15 +4541,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>1015</v>
       </c>
@@ -3510,8 +4565,11 @@
       <c r="F1">
         <v>1071</v>
       </c>
+      <c r="G1">
+        <v>1018</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3530,8 +4588,11 @@
       <c r="F2">
         <v>4.4900000000000002E-2</v>
       </c>
+      <c r="G2">
+        <v>1.2999999999999999E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3550,8 +4611,11 @@
       <c r="F3">
         <v>0.14549999999999999</v>
       </c>
+      <c r="G3">
+        <v>5.0999999999999997E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3570,8 +4634,40 @@
       <c r="F4">
         <v>0.13389999999999999</v>
       </c>
+      <c r="G4">
+        <v>4.4200000000000003E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(B2:B4)</f>
+        <v>5.8333333333333327E-2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:G5" si="0">AVERAGE(C2:C4)</f>
+        <v>6.376666666666668E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.16523333333333334</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.10809999999999999</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>3.606666666666667E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3591,7 +4687,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3610,8 +4706,11 @@
       <c r="F8">
         <v>5.63</v>
       </c>
+      <c r="G8">
+        <v>20.3</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3629,6 +4728,52 @@
       </c>
       <c r="F9">
         <v>11.41</v>
+      </c>
+      <c r="G9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>81</v>
+      </c>
+      <c r="D10">
+        <v>65</v>
+      </c>
+      <c r="E10">
+        <v>66</v>
+      </c>
+      <c r="G10">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>